<commit_message>
AutomationTest-FinalProject: Remove Unused Import
</commit_message>
<xml_diff>
--- a/src/data/ManualTestCases.xlsx
+++ b/src/data/ManualTestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\automation-test-group1\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="AddProject" sheetId="1" r:id="rId1"/>
@@ -1540,9 +1540,96 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1552,19 +1639,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1573,148 +1681,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="41" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2040,7 +2040,7 @@
   </sheetPr>
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -2058,18 +2058,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -2116,33 +2116,33 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="53">
+      <c r="A5" s="61">
         <v>1</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="9">
@@ -2157,14 +2157,14 @@
       <c r="I5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="70"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="60"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="88"/>
       <c r="F6" s="12">
         <v>2</v>
       </c>
@@ -2177,14 +2177,14 @@
       <c r="I6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="71"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="61"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="12">
         <v>3</v>
       </c>
@@ -2195,14 +2195,14 @@
       <c r="I7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="71"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="61"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="12">
         <v>4</v>
       </c>
@@ -2213,14 +2213,14 @@
       <c r="I8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="71"/>
+      <c r="J8" s="57"/>
     </row>
     <row r="9" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="61"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="12">
         <v>5</v>
       </c>
@@ -2231,76 +2231,76 @@
       <c r="I9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="71"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="98">
+      <c r="A10" s="83"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="77">
         <v>6</v>
       </c>
-      <c r="G10" s="77" t="s">
+      <c r="G10" s="53" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="77" t="s">
+      <c r="I10" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="71"/>
+      <c r="J10" s="57"/>
     </row>
     <row r="11" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="78"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="78"/>
-      <c r="J11" s="71"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="57"/>
     </row>
     <row r="12" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="78"/>
-      <c r="J12" s="71"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="97"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="97"/>
-      <c r="J13" s="71"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="61"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="89"/>
       <c r="F14" s="13">
         <v>7</v>
       </c>
@@ -2311,22 +2311,22 @@
       <c r="I14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="71"/>
+      <c r="J14" s="57"/>
     </row>
     <row r="15" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="92">
+      <c r="A15" s="75">
         <v>2</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="9">
@@ -2341,14 +2341,14 @@
       <c r="I15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="70"/>
+      <c r="J15" s="56"/>
     </row>
     <row r="16" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="93"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="60"/>
+      <c r="A16" s="76"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="88"/>
       <c r="F16" s="12">
         <v>2</v>
       </c>
@@ -2361,14 +2361,14 @@
       <c r="I16" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="71"/>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="93"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="61"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="89"/>
       <c r="F17" s="12">
         <v>3</v>
       </c>
@@ -2379,14 +2379,14 @@
       <c r="I17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="71"/>
+      <c r="J17" s="57"/>
     </row>
     <row r="18" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="93"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="61"/>
+      <c r="A18" s="76"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="89"/>
       <c r="F18" s="12">
         <v>4</v>
       </c>
@@ -2397,14 +2397,14 @@
       <c r="I18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="71"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="93"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="61"/>
+      <c r="A19" s="76"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="89"/>
       <c r="F19" s="12">
         <v>5</v>
       </c>
@@ -2415,76 +2415,76 @@
       <c r="I19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="71"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="93"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="98">
+      <c r="A20" s="76"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="77">
         <v>6</v>
       </c>
-      <c r="G20" s="77" t="s">
+      <c r="G20" s="53" t="s">
         <v>38</v>
       </c>
       <c r="H20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="77" t="s">
+      <c r="I20" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="71"/>
+      <c r="J20" s="57"/>
     </row>
     <row r="21" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="93"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="78"/>
+      <c r="A21" s="76"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="78"/>
-      <c r="J21" s="71"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="57"/>
     </row>
     <row r="22" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="93"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="78"/>
+      <c r="A22" s="76"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="78"/>
-      <c r="J22" s="71"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="57"/>
     </row>
     <row r="23" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="93"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="97"/>
+      <c r="A23" s="76"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="55"/>
       <c r="H23" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I23" s="97"/>
-      <c r="J23" s="71"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="57"/>
     </row>
     <row r="24" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="93"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="61"/>
+      <c r="A24" s="76"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="89"/>
       <c r="F24" s="13">
         <v>7</v>
       </c>
@@ -2495,20 +2495,20 @@
       <c r="I24" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="71"/>
+      <c r="J24" s="57"/>
     </row>
     <row r="25" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="92">
+      <c r="A25" s="75">
         <v>3</v>
       </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="53" t="s">
+      <c r="B25" s="85"/>
+      <c r="C25" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="9">
@@ -2523,14 +2523,14 @@
       <c r="I25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="70"/>
+      <c r="J25" s="56"/>
     </row>
     <row r="26" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="93"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="60"/>
+      <c r="A26" s="76"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="88"/>
       <c r="F26" s="15">
         <v>2</v>
       </c>
@@ -2543,14 +2543,14 @@
       <c r="I26" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="71"/>
+      <c r="J26" s="57"/>
     </row>
     <row r="27" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="93"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="61"/>
+      <c r="A27" s="76"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="89"/>
       <c r="F27" s="15">
         <v>3</v>
       </c>
@@ -2561,14 +2561,14 @@
       <c r="I27" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="71"/>
+      <c r="J27" s="57"/>
     </row>
     <row r="28" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="93"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="61"/>
+      <c r="A28" s="76"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="89"/>
       <c r="F28" s="15">
         <v>4</v>
       </c>
@@ -2579,14 +2579,14 @@
       <c r="I28" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="71"/>
+      <c r="J28" s="57"/>
     </row>
     <row r="29" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="93"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="61"/>
+      <c r="A29" s="76"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="89"/>
       <c r="F29" s="15">
         <v>5</v>
       </c>
@@ -2597,76 +2597,76 @@
       <c r="I29" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J29" s="71"/>
+      <c r="J29" s="57"/>
     </row>
     <row r="30" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="93"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="96">
+      <c r="A30" s="76"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="58">
         <v>6</v>
       </c>
-      <c r="G30" s="94" t="s">
+      <c r="G30" s="59" t="s">
         <v>38</v>
       </c>
       <c r="H30" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="77" t="s">
+      <c r="I30" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="71"/>
+      <c r="J30" s="57"/>
     </row>
     <row r="31" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="93"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="94"/>
+      <c r="A31" s="76"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
       <c r="H31" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="78"/>
-      <c r="J31" s="71"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="57"/>
     </row>
     <row r="32" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="93"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="94"/>
+      <c r="A32" s="76"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
       <c r="H32" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="78"/>
-      <c r="J32" s="71"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="57"/>
     </row>
     <row r="33" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="93"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="94"/>
+      <c r="A33" s="76"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="59"/>
       <c r="H33" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I33" s="97"/>
-      <c r="J33" s="71"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="57"/>
     </row>
     <row r="34" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="93"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="61"/>
+      <c r="A34" s="76"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="89"/>
       <c r="F34" s="15">
         <v>7</v>
       </c>
@@ -2677,20 +2677,20 @@
       <c r="I34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="71"/>
+      <c r="J34" s="57"/>
     </row>
     <row r="35" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="92">
+      <c r="A35" s="75">
         <v>4</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="53" t="s">
+      <c r="B35" s="85"/>
+      <c r="C35" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="64" t="s">
+      <c r="D35" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="59" t="s">
+      <c r="E35" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="9">
@@ -2705,14 +2705,14 @@
       <c r="I35" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="70"/>
+      <c r="J35" s="56"/>
     </row>
     <row r="36" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="93"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="60"/>
+      <c r="A36" s="76"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="88"/>
       <c r="F36" s="15">
         <v>2</v>
       </c>
@@ -2725,14 +2725,14 @@
       <c r="I36" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="71"/>
+      <c r="J36" s="57"/>
     </row>
     <row r="37" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="93"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="61"/>
+      <c r="A37" s="76"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="89"/>
       <c r="F37" s="15">
         <v>3</v>
       </c>
@@ -2743,14 +2743,14 @@
       <c r="I37" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="71"/>
+      <c r="J37" s="57"/>
     </row>
     <row r="38" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="93"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="61"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="89"/>
       <c r="F38" s="15">
         <v>4</v>
       </c>
@@ -2761,14 +2761,14 @@
       <c r="I38" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J38" s="71"/>
+      <c r="J38" s="57"/>
     </row>
     <row r="39" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="93"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="61"/>
+      <c r="A39" s="76"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="89"/>
       <c r="F39" s="15">
         <v>5</v>
       </c>
@@ -2779,76 +2779,76 @@
       <c r="I39" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J39" s="71"/>
+      <c r="J39" s="57"/>
     </row>
     <row r="40" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="93"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="96">
+      <c r="A40" s="76"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="58">
         <v>6</v>
       </c>
-      <c r="G40" s="94" t="s">
+      <c r="G40" s="59" t="s">
         <v>38</v>
       </c>
       <c r="H40" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I40" s="77" t="s">
+      <c r="I40" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J40" s="71"/>
+      <c r="J40" s="57"/>
     </row>
     <row r="41" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="93"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="96"/>
-      <c r="G41" s="94"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="59"/>
       <c r="H41" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="I41" s="78"/>
-      <c r="J41" s="71"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="57"/>
     </row>
     <row r="42" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="93"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="94"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="59"/>
       <c r="H42" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I42" s="78"/>
-      <c r="J42" s="71"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="57"/>
     </row>
     <row r="43" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="93"/>
-      <c r="B43" s="56"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="96"/>
-      <c r="G43" s="94"/>
+      <c r="A43" s="76"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="59"/>
       <c r="H43" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I43" s="97"/>
-      <c r="J43" s="71"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="57"/>
     </row>
     <row r="44" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="93"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="61"/>
+      <c r="A44" s="76"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="89"/>
       <c r="F44" s="15">
         <v>7</v>
       </c>
@@ -2859,20 +2859,20 @@
       <c r="I44" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J44" s="71"/>
+      <c r="J44" s="57"/>
     </row>
     <row r="45" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="92">
+      <c r="A45" s="75">
         <v>5</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="53" t="s">
+      <c r="B45" s="85"/>
+      <c r="C45" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="64" t="s">
+      <c r="D45" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="E45" s="59" t="s">
+      <c r="E45" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F45" s="9">
@@ -2887,14 +2887,14 @@
       <c r="I45" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J45" s="70"/>
+      <c r="J45" s="56"/>
     </row>
     <row r="46" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="93"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="65"/>
-      <c r="E46" s="60"/>
+      <c r="A46" s="76"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="88"/>
       <c r="F46" s="15">
         <v>2</v>
       </c>
@@ -2907,14 +2907,14 @@
       <c r="I46" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J46" s="71"/>
+      <c r="J46" s="57"/>
     </row>
     <row r="47" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="93"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="61"/>
+      <c r="A47" s="76"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="89"/>
       <c r="F47" s="15">
         <v>3</v>
       </c>
@@ -2925,14 +2925,14 @@
       <c r="I47" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J47" s="71"/>
+      <c r="J47" s="57"/>
     </row>
     <row r="48" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="93"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="61"/>
+      <c r="A48" s="76"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="89"/>
       <c r="F48" s="15">
         <v>4</v>
       </c>
@@ -2943,14 +2943,14 @@
       <c r="I48" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J48" s="71"/>
+      <c r="J48" s="57"/>
     </row>
     <row r="49" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="93"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="66"/>
-      <c r="E49" s="61"/>
+      <c r="A49" s="76"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="89"/>
       <c r="F49" s="15">
         <v>5</v>
       </c>
@@ -2961,76 +2961,76 @@
       <c r="I49" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J49" s="71"/>
+      <c r="J49" s="57"/>
     </row>
     <row r="50" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="93"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="66"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="96">
+      <c r="A50" s="76"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="58">
         <v>6</v>
       </c>
-      <c r="G50" s="94" t="s">
+      <c r="G50" s="59" t="s">
         <v>38</v>
       </c>
       <c r="H50" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I50" s="77" t="s">
+      <c r="I50" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J50" s="71"/>
+      <c r="J50" s="57"/>
     </row>
     <row r="51" spans="1:10" ht="117.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="93"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="96"/>
-      <c r="G51" s="94"/>
+      <c r="A51" s="76"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="59"/>
       <c r="H51" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="I51" s="78"/>
-      <c r="J51" s="71"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="57"/>
     </row>
     <row r="52" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="93"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="94"/>
+      <c r="A52" s="76"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="59"/>
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="78"/>
-      <c r="J52" s="71"/>
+      <c r="I52" s="54"/>
+      <c r="J52" s="57"/>
     </row>
     <row r="53" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="93"/>
-      <c r="B53" s="56"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="66"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="96"/>
-      <c r="G53" s="94"/>
+      <c r="A53" s="76"/>
+      <c r="B53" s="85"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="59"/>
       <c r="H53" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I53" s="97"/>
-      <c r="J53" s="71"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="57"/>
     </row>
     <row r="54" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="93"/>
-      <c r="B54" s="56"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="66"/>
-      <c r="E54" s="61"/>
+      <c r="A54" s="76"/>
+      <c r="B54" s="85"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="89"/>
       <c r="F54" s="15">
         <v>7</v>
       </c>
@@ -3041,20 +3041,20 @@
       <c r="I54" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J54" s="71"/>
+      <c r="J54" s="57"/>
     </row>
     <row r="55" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="92">
+      <c r="A55" s="75">
         <v>6</v>
       </c>
-      <c r="B55" s="56"/>
-      <c r="C55" s="53" t="s">
+      <c r="B55" s="85"/>
+      <c r="C55" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="64" t="s">
+      <c r="D55" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E55" s="59" t="s">
+      <c r="E55" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F55" s="9">
@@ -3069,14 +3069,14 @@
       <c r="I55" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J55" s="70"/>
+      <c r="J55" s="56"/>
     </row>
     <row r="56" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="93"/>
-      <c r="B56" s="56"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="65"/>
-      <c r="E56" s="60"/>
+      <c r="A56" s="76"/>
+      <c r="B56" s="85"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="88"/>
       <c r="F56" s="15">
         <v>2</v>
       </c>
@@ -3089,14 +3089,14 @@
       <c r="I56" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J56" s="71"/>
+      <c r="J56" s="57"/>
     </row>
     <row r="57" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="93"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="61"/>
+      <c r="A57" s="76"/>
+      <c r="B57" s="85"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="89"/>
       <c r="F57" s="15">
         <v>3</v>
       </c>
@@ -3107,14 +3107,14 @@
       <c r="I57" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J57" s="71"/>
+      <c r="J57" s="57"/>
     </row>
     <row r="58" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="93"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="61"/>
+      <c r="A58" s="76"/>
+      <c r="B58" s="85"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="89"/>
       <c r="F58" s="15">
         <v>4</v>
       </c>
@@ -3125,14 +3125,14 @@
       <c r="I58" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J58" s="71"/>
+      <c r="J58" s="57"/>
     </row>
     <row r="59" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="93"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="61"/>
+      <c r="A59" s="76"/>
+      <c r="B59" s="85"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="89"/>
       <c r="F59" s="15">
         <v>5</v>
       </c>
@@ -3143,76 +3143,76 @@
       <c r="I59" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J59" s="71"/>
+      <c r="J59" s="57"/>
     </row>
     <row r="60" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="93"/>
-      <c r="B60" s="56"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="66"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="96">
+      <c r="A60" s="76"/>
+      <c r="B60" s="85"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="89"/>
+      <c r="F60" s="58">
         <v>6</v>
       </c>
-      <c r="G60" s="94" t="s">
+      <c r="G60" s="59" t="s">
         <v>38</v>
       </c>
       <c r="H60" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I60" s="77" t="s">
+      <c r="I60" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J60" s="71"/>
+      <c r="J60" s="57"/>
     </row>
     <row r="61" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="93"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="96"/>
-      <c r="G61" s="94"/>
+      <c r="A61" s="76"/>
+      <c r="B61" s="85"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="59"/>
       <c r="H61" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I61" s="78"/>
-      <c r="J61" s="71"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="57"/>
     </row>
     <row r="62" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="93"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="66"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="96"/>
-      <c r="G62" s="94"/>
+      <c r="A62" s="76"/>
+      <c r="B62" s="85"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="89"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="59"/>
       <c r="H62" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I62" s="78"/>
-      <c r="J62" s="71"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="57"/>
     </row>
     <row r="63" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="93"/>
-      <c r="B63" s="56"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="61"/>
-      <c r="F63" s="96"/>
-      <c r="G63" s="94"/>
+      <c r="A63" s="76"/>
+      <c r="B63" s="85"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="89"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="59"/>
       <c r="H63" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I63" s="95"/>
-      <c r="J63" s="71"/>
+      <c r="I63" s="60"/>
+      <c r="J63" s="57"/>
     </row>
     <row r="64" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="93"/>
-      <c r="B64" s="56"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="61"/>
+      <c r="A64" s="76"/>
+      <c r="B64" s="85"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="65"/>
+      <c r="E64" s="89"/>
       <c r="F64" s="15">
         <v>7</v>
       </c>
@@ -3223,20 +3223,20 @@
       <c r="I64" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J64" s="71"/>
+      <c r="J64" s="57"/>
     </row>
     <row r="65" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="92">
+      <c r="A65" s="75">
         <v>7</v>
       </c>
-      <c r="B65" s="56"/>
-      <c r="C65" s="53" t="s">
+      <c r="B65" s="85"/>
+      <c r="C65" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="D65" s="64" t="s">
+      <c r="D65" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="E65" s="59" t="s">
+      <c r="E65" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F65" s="9">
@@ -3251,14 +3251,14 @@
       <c r="I65" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J65" s="70"/>
+      <c r="J65" s="56"/>
     </row>
     <row r="66" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="93"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="65"/>
-      <c r="E66" s="60"/>
+      <c r="A66" s="76"/>
+      <c r="B66" s="85"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="88"/>
       <c r="F66" s="15">
         <v>2</v>
       </c>
@@ -3271,14 +3271,14 @@
       <c r="I66" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J66" s="71"/>
+      <c r="J66" s="57"/>
     </row>
     <row r="67" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="93"/>
-      <c r="B67" s="56"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="66"/>
-      <c r="E67" s="61"/>
+      <c r="A67" s="76"/>
+      <c r="B67" s="85"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="89"/>
       <c r="F67" s="15">
         <v>3</v>
       </c>
@@ -3289,14 +3289,14 @@
       <c r="I67" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J67" s="71"/>
+      <c r="J67" s="57"/>
     </row>
     <row r="68" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="93"/>
-      <c r="B68" s="56"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="66"/>
-      <c r="E68" s="61"/>
+      <c r="A68" s="76"/>
+      <c r="B68" s="85"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="89"/>
       <c r="F68" s="15">
         <v>4</v>
       </c>
@@ -3307,14 +3307,14 @@
       <c r="I68" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J68" s="71"/>
+      <c r="J68" s="57"/>
     </row>
     <row r="69" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="93"/>
-      <c r="B69" s="56"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="66"/>
-      <c r="E69" s="61"/>
+      <c r="A69" s="76"/>
+      <c r="B69" s="85"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="65"/>
+      <c r="E69" s="89"/>
       <c r="F69" s="15">
         <v>5</v>
       </c>
@@ -3325,76 +3325,76 @@
       <c r="I69" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J69" s="71"/>
+      <c r="J69" s="57"/>
     </row>
     <row r="70" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="93"/>
-      <c r="B70" s="56"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="66"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="96">
+      <c r="A70" s="76"/>
+      <c r="B70" s="85"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="65"/>
+      <c r="E70" s="89"/>
+      <c r="F70" s="58">
         <v>6</v>
       </c>
-      <c r="G70" s="94" t="s">
+      <c r="G70" s="59" t="s">
         <v>38</v>
       </c>
       <c r="H70" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I70" s="77" t="s">
+      <c r="I70" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J70" s="71"/>
+      <c r="J70" s="57"/>
     </row>
     <row r="71" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="93"/>
-      <c r="B71" s="56"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="66"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="96"/>
-      <c r="G71" s="94"/>
+      <c r="A71" s="76"/>
+      <c r="B71" s="85"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="65"/>
+      <c r="E71" s="89"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="59"/>
       <c r="H71" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I71" s="78"/>
-      <c r="J71" s="71"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="57"/>
     </row>
     <row r="72" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="93"/>
-      <c r="B72" s="56"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="66"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="96"/>
-      <c r="G72" s="94"/>
+      <c r="A72" s="76"/>
+      <c r="B72" s="85"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="65"/>
+      <c r="E72" s="89"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="59"/>
       <c r="H72" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I72" s="78"/>
-      <c r="J72" s="71"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="57"/>
     </row>
     <row r="73" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="93"/>
-      <c r="B73" s="56"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="96"/>
-      <c r="G73" s="94"/>
+      <c r="A73" s="76"/>
+      <c r="B73" s="85"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="89"/>
+      <c r="F73" s="58"/>
+      <c r="G73" s="59"/>
       <c r="H73" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I73" s="95"/>
-      <c r="J73" s="71"/>
+      <c r="I73" s="60"/>
+      <c r="J73" s="57"/>
     </row>
     <row r="74" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="93"/>
-      <c r="B74" s="57"/>
-      <c r="C74" s="58"/>
-      <c r="D74" s="66"/>
-      <c r="E74" s="61"/>
+      <c r="A74" s="76"/>
+      <c r="B74" s="90"/>
+      <c r="C74" s="62"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="89"/>
       <c r="F74" s="15">
         <v>7</v>
       </c>
@@ -3405,22 +3405,22 @@
       <c r="I74" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J74" s="71"/>
+      <c r="J74" s="57"/>
     </row>
     <row r="75" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="53">
+      <c r="A75" s="61">
         <v>8</v>
       </c>
-      <c r="B75" s="55" t="s">
+      <c r="B75" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="C75" s="55" t="s">
+      <c r="C75" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="D75" s="86" t="s">
+      <c r="D75" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E75" s="89" t="s">
+      <c r="E75" s="94" t="s">
         <v>60</v>
       </c>
       <c r="F75" s="9">
@@ -3435,14 +3435,14 @@
       <c r="I75" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J75" s="70"/>
+      <c r="J75" s="56"/>
     </row>
     <row r="76" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="54"/>
-      <c r="B76" s="85"/>
-      <c r="C76" s="85"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="90"/>
+      <c r="A76" s="83"/>
+      <c r="B76" s="86"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="95"/>
       <c r="F76" s="15">
         <v>2</v>
       </c>
@@ -3455,14 +3455,14 @@
       <c r="I76" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J76" s="71"/>
+      <c r="J76" s="57"/>
     </row>
     <row r="77" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="54"/>
-      <c r="B77" s="85"/>
-      <c r="C77" s="85"/>
-      <c r="D77" s="88"/>
-      <c r="E77" s="91"/>
+      <c r="A77" s="83"/>
+      <c r="B77" s="86"/>
+      <c r="C77" s="86"/>
+      <c r="D77" s="93"/>
+      <c r="E77" s="96"/>
       <c r="F77" s="15">
         <v>3</v>
       </c>
@@ -3473,14 +3473,14 @@
       <c r="I77" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J77" s="71"/>
+      <c r="J77" s="57"/>
     </row>
     <row r="78" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="54"/>
-      <c r="B78" s="85"/>
-      <c r="C78" s="85"/>
-      <c r="D78" s="88"/>
-      <c r="E78" s="91"/>
+      <c r="A78" s="83"/>
+      <c r="B78" s="86"/>
+      <c r="C78" s="86"/>
+      <c r="D78" s="93"/>
+      <c r="E78" s="96"/>
       <c r="F78" s="15">
         <v>4</v>
       </c>
@@ -3491,14 +3491,14 @@
       <c r="I78" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J78" s="71"/>
+      <c r="J78" s="57"/>
     </row>
     <row r="79" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="54"/>
-      <c r="B79" s="85"/>
-      <c r="C79" s="85"/>
-      <c r="D79" s="88"/>
-      <c r="E79" s="91"/>
+      <c r="A79" s="83"/>
+      <c r="B79" s="86"/>
+      <c r="C79" s="86"/>
+      <c r="D79" s="93"/>
+      <c r="E79" s="96"/>
       <c r="F79" s="15">
         <v>5</v>
       </c>
@@ -3509,14 +3509,14 @@
       <c r="I79" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J79" s="71"/>
+      <c r="J79" s="57"/>
     </row>
     <row r="80" spans="1:10" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="54"/>
-      <c r="B80" s="85"/>
-      <c r="C80" s="85"/>
-      <c r="D80" s="88"/>
-      <c r="E80" s="91"/>
+      <c r="A80" s="83"/>
+      <c r="B80" s="86"/>
+      <c r="C80" s="86"/>
+      <c r="D80" s="93"/>
+      <c r="E80" s="96"/>
       <c r="F80" s="18">
         <v>6</v>
       </c>
@@ -3529,22 +3529,22 @@
       <c r="I80" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J80" s="71"/>
+      <c r="J80" s="57"/>
     </row>
     <row r="81" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="53">
+      <c r="A81" s="61">
         <v>9</v>
       </c>
-      <c r="B81" s="55" t="s">
+      <c r="B81" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="C81" s="55" t="s">
+      <c r="C81" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="86" t="s">
+      <c r="D81" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E81" s="89" t="s">
+      <c r="E81" s="94" t="s">
         <v>66</v>
       </c>
       <c r="F81" s="9">
@@ -3559,14 +3559,14 @@
       <c r="I81" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="70"/>
+      <c r="J81" s="56"/>
     </row>
     <row r="82" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="54"/>
-      <c r="B82" s="85"/>
-      <c r="C82" s="85"/>
-      <c r="D82" s="87"/>
-      <c r="E82" s="90"/>
+      <c r="A82" s="83"/>
+      <c r="B82" s="86"/>
+      <c r="C82" s="86"/>
+      <c r="D82" s="92"/>
+      <c r="E82" s="95"/>
       <c r="F82" s="15">
         <v>2</v>
       </c>
@@ -3579,14 +3579,14 @@
       <c r="I82" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J82" s="71"/>
+      <c r="J82" s="57"/>
     </row>
     <row r="83" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="54"/>
-      <c r="B83" s="85"/>
-      <c r="C83" s="85"/>
-      <c r="D83" s="88"/>
-      <c r="E83" s="91"/>
+      <c r="A83" s="83"/>
+      <c r="B83" s="86"/>
+      <c r="C83" s="86"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="96"/>
       <c r="F83" s="15">
         <v>3</v>
       </c>
@@ -3597,14 +3597,14 @@
       <c r="I83" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J83" s="71"/>
+      <c r="J83" s="57"/>
     </row>
     <row r="84" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="54"/>
-      <c r="B84" s="85"/>
-      <c r="C84" s="85"/>
-      <c r="D84" s="88"/>
-      <c r="E84" s="91"/>
+      <c r="A84" s="83"/>
+      <c r="B84" s="86"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="93"/>
+      <c r="E84" s="96"/>
       <c r="F84" s="15">
         <v>4</v>
       </c>
@@ -3615,14 +3615,14 @@
       <c r="I84" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J84" s="71"/>
+      <c r="J84" s="57"/>
     </row>
     <row r="85" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="54"/>
-      <c r="B85" s="85"/>
-      <c r="C85" s="85"/>
-      <c r="D85" s="88"/>
-      <c r="E85" s="91"/>
+      <c r="A85" s="83"/>
+      <c r="B85" s="86"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="93"/>
+      <c r="E85" s="96"/>
       <c r="F85" s="15">
         <v>5</v>
       </c>
@@ -3633,14 +3633,14 @@
       <c r="I85" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J85" s="71"/>
+      <c r="J85" s="57"/>
     </row>
     <row r="86" spans="1:10" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="54"/>
-      <c r="B86" s="85"/>
-      <c r="C86" s="85"/>
-      <c r="D86" s="88"/>
-      <c r="E86" s="91"/>
+      <c r="A86" s="83"/>
+      <c r="B86" s="86"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="93"/>
+      <c r="E86" s="96"/>
       <c r="F86" s="18">
         <v>6</v>
       </c>
@@ -3653,22 +3653,22 @@
       <c r="I86" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J86" s="71"/>
+      <c r="J86" s="57"/>
     </row>
     <row r="87" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="53">
+      <c r="A87" s="61">
         <v>10</v>
       </c>
-      <c r="B87" s="55" t="s">
+      <c r="B87" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="C87" s="53" t="s">
+      <c r="C87" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="D87" s="64" t="s">
+      <c r="D87" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="E87" s="59" t="s">
+      <c r="E87" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F87" s="9">
@@ -3683,14 +3683,14 @@
       <c r="I87" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J87" s="70"/>
+      <c r="J87" s="56"/>
     </row>
     <row r="88" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="54"/>
-      <c r="B88" s="56"/>
-      <c r="C88" s="58"/>
-      <c r="D88" s="65"/>
-      <c r="E88" s="60"/>
+      <c r="A88" s="83"/>
+      <c r="B88" s="85"/>
+      <c r="C88" s="62"/>
+      <c r="D88" s="64"/>
+      <c r="E88" s="88"/>
       <c r="F88" s="15">
         <v>2</v>
       </c>
@@ -3703,14 +3703,14 @@
       <c r="I88" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J88" s="71"/>
+      <c r="J88" s="57"/>
     </row>
     <row r="89" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="54"/>
-      <c r="B89" s="56"/>
-      <c r="C89" s="58"/>
-      <c r="D89" s="66"/>
-      <c r="E89" s="61"/>
+      <c r="A89" s="83"/>
+      <c r="B89" s="85"/>
+      <c r="C89" s="62"/>
+      <c r="D89" s="65"/>
+      <c r="E89" s="89"/>
       <c r="F89" s="15">
         <v>3</v>
       </c>
@@ -3721,14 +3721,14 @@
       <c r="I89" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J89" s="71"/>
+      <c r="J89" s="57"/>
     </row>
     <row r="90" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="54"/>
-      <c r="B90" s="56"/>
-      <c r="C90" s="58"/>
-      <c r="D90" s="66"/>
-      <c r="E90" s="61"/>
+      <c r="A90" s="83"/>
+      <c r="B90" s="85"/>
+      <c r="C90" s="62"/>
+      <c r="D90" s="65"/>
+      <c r="E90" s="89"/>
       <c r="F90" s="15">
         <v>4</v>
       </c>
@@ -3739,14 +3739,14 @@
       <c r="I90" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J90" s="71"/>
+      <c r="J90" s="57"/>
     </row>
     <row r="91" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A91" s="54"/>
-      <c r="B91" s="56"/>
-      <c r="C91" s="58"/>
-      <c r="D91" s="66"/>
-      <c r="E91" s="61"/>
+      <c r="A91" s="83"/>
+      <c r="B91" s="85"/>
+      <c r="C91" s="62"/>
+      <c r="D91" s="65"/>
+      <c r="E91" s="89"/>
       <c r="F91" s="15">
         <v>5</v>
       </c>
@@ -3757,14 +3757,14 @@
       <c r="I91" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J91" s="71"/>
+      <c r="J91" s="57"/>
     </row>
     <row r="92" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="54"/>
-      <c r="B92" s="56"/>
-      <c r="C92" s="58"/>
-      <c r="D92" s="66"/>
-      <c r="E92" s="61"/>
+      <c r="A92" s="83"/>
+      <c r="B92" s="85"/>
+      <c r="C92" s="62"/>
+      <c r="D92" s="65"/>
+      <c r="E92" s="89"/>
       <c r="F92" s="17">
         <v>6</v>
       </c>
@@ -3772,63 +3772,63 @@
         <v>71</v>
       </c>
       <c r="H92" s="31"/>
-      <c r="I92" s="77" t="s">
+      <c r="I92" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="J92" s="71"/>
+      <c r="J92" s="57"/>
     </row>
     <row r="93" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="54"/>
-      <c r="B93" s="56"/>
-      <c r="C93" s="58"/>
-      <c r="D93" s="66"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="73">
+      <c r="A93" s="83"/>
+      <c r="B93" s="85"/>
+      <c r="C93" s="62"/>
+      <c r="D93" s="65"/>
+      <c r="E93" s="89"/>
+      <c r="F93" s="67">
         <v>7</v>
       </c>
-      <c r="G93" s="82" t="s">
+      <c r="G93" s="71" t="s">
         <v>73</v>
       </c>
       <c r="H93" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I93" s="78"/>
-      <c r="J93" s="71"/>
+      <c r="I93" s="54"/>
+      <c r="J93" s="57"/>
     </row>
     <row r="94" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A94" s="54"/>
-      <c r="B94" s="56"/>
-      <c r="C94" s="58"/>
-      <c r="D94" s="66"/>
-      <c r="E94" s="61"/>
-      <c r="F94" s="74"/>
-      <c r="G94" s="83"/>
+      <c r="A94" s="83"/>
+      <c r="B94" s="85"/>
+      <c r="C94" s="62"/>
+      <c r="D94" s="65"/>
+      <c r="E94" s="89"/>
+      <c r="F94" s="68"/>
+      <c r="G94" s="72"/>
       <c r="H94" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="I94" s="78"/>
-      <c r="J94" s="71"/>
+      <c r="I94" s="54"/>
+      <c r="J94" s="57"/>
     </row>
     <row r="95" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="54"/>
-      <c r="B95" s="56"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="66"/>
-      <c r="E95" s="61"/>
-      <c r="F95" s="81"/>
-      <c r="G95" s="84"/>
+      <c r="A95" s="83"/>
+      <c r="B95" s="85"/>
+      <c r="C95" s="62"/>
+      <c r="D95" s="65"/>
+      <c r="E95" s="89"/>
+      <c r="F95" s="74"/>
+      <c r="G95" s="73"/>
       <c r="H95" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I95" s="78"/>
-      <c r="J95" s="71"/>
+      <c r="I95" s="54"/>
+      <c r="J95" s="57"/>
     </row>
     <row r="96" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="54"/>
-      <c r="B96" s="56"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="66"/>
-      <c r="E96" s="61"/>
+      <c r="A96" s="83"/>
+      <c r="B96" s="85"/>
+      <c r="C96" s="62"/>
+      <c r="D96" s="65"/>
+      <c r="E96" s="89"/>
       <c r="F96" s="21">
         <v>8</v>
       </c>
@@ -3836,21 +3836,21 @@
         <v>33</v>
       </c>
       <c r="H96" s="28"/>
-      <c r="I96" s="78"/>
-      <c r="J96" s="71"/>
+      <c r="I96" s="54"/>
+      <c r="J96" s="57"/>
     </row>
     <row r="97" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="53">
+      <c r="A97" s="61">
         <v>11</v>
       </c>
-      <c r="B97" s="56"/>
-      <c r="C97" s="53" t="s">
+      <c r="B97" s="85"/>
+      <c r="C97" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="D97" s="64" t="s">
+      <c r="D97" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="E97" s="59" t="s">
+      <c r="E97" s="87" t="s">
         <v>15</v>
       </c>
       <c r="F97" s="9">
@@ -3865,14 +3865,14 @@
       <c r="I97" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J97" s="70"/>
+      <c r="J97" s="56"/>
     </row>
     <row r="98" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="54"/>
-      <c r="B98" s="56"/>
-      <c r="C98" s="58"/>
-      <c r="D98" s="65"/>
-      <c r="E98" s="60"/>
+      <c r="A98" s="83"/>
+      <c r="B98" s="85"/>
+      <c r="C98" s="62"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="88"/>
       <c r="F98" s="15">
         <v>2</v>
       </c>
@@ -3885,14 +3885,14 @@
       <c r="I98" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J98" s="71"/>
+      <c r="J98" s="57"/>
     </row>
     <row r="99" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A99" s="54"/>
-      <c r="B99" s="56"/>
-      <c r="C99" s="58"/>
-      <c r="D99" s="66"/>
-      <c r="E99" s="61"/>
+      <c r="A99" s="83"/>
+      <c r="B99" s="85"/>
+      <c r="C99" s="62"/>
+      <c r="D99" s="65"/>
+      <c r="E99" s="89"/>
       <c r="F99" s="15">
         <v>3</v>
       </c>
@@ -3903,14 +3903,14 @@
       <c r="I99" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J99" s="71"/>
+      <c r="J99" s="57"/>
     </row>
     <row r="100" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="54"/>
-      <c r="B100" s="56"/>
-      <c r="C100" s="58"/>
-      <c r="D100" s="66"/>
-      <c r="E100" s="61"/>
+      <c r="A100" s="83"/>
+      <c r="B100" s="85"/>
+      <c r="C100" s="62"/>
+      <c r="D100" s="65"/>
+      <c r="E100" s="89"/>
       <c r="F100" s="15">
         <v>4</v>
       </c>
@@ -3921,14 +3921,14 @@
       <c r="I100" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J100" s="71"/>
+      <c r="J100" s="57"/>
     </row>
     <row r="101" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A101" s="54"/>
-      <c r="B101" s="56"/>
-      <c r="C101" s="58"/>
-      <c r="D101" s="66"/>
-      <c r="E101" s="61"/>
+      <c r="A101" s="83"/>
+      <c r="B101" s="85"/>
+      <c r="C101" s="62"/>
+      <c r="D101" s="65"/>
+      <c r="E101" s="89"/>
       <c r="F101" s="15">
         <v>5</v>
       </c>
@@ -3939,62 +3939,62 @@
       <c r="I101" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J101" s="71"/>
+      <c r="J101" s="57"/>
     </row>
     <row r="102" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="54"/>
-      <c r="B102" s="56"/>
-      <c r="C102" s="58"/>
-      <c r="D102" s="66"/>
-      <c r="E102" s="61"/>
-      <c r="F102" s="73">
+      <c r="A102" s="83"/>
+      <c r="B102" s="85"/>
+      <c r="C102" s="62"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="89"/>
+      <c r="F102" s="67">
         <v>6</v>
       </c>
-      <c r="G102" s="75" t="s">
+      <c r="G102" s="69" t="s">
         <v>77</v>
       </c>
       <c r="H102" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="I102" s="77" t="s">
+      <c r="I102" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="J102" s="71"/>
+      <c r="J102" s="57"/>
     </row>
     <row r="103" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="54"/>
-      <c r="B103" s="56"/>
-      <c r="C103" s="58"/>
-      <c r="D103" s="66"/>
-      <c r="E103" s="61"/>
-      <c r="F103" s="74"/>
-      <c r="G103" s="76"/>
+      <c r="A103" s="83"/>
+      <c r="B103" s="85"/>
+      <c r="C103" s="62"/>
+      <c r="D103" s="65"/>
+      <c r="E103" s="89"/>
+      <c r="F103" s="68"/>
+      <c r="G103" s="70"/>
       <c r="H103" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I103" s="78"/>
-      <c r="J103" s="71"/>
+      <c r="I103" s="54"/>
+      <c r="J103" s="57"/>
     </row>
     <row r="104" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="54"/>
-      <c r="B104" s="56"/>
-      <c r="C104" s="58"/>
-      <c r="D104" s="66"/>
-      <c r="E104" s="61"/>
-      <c r="F104" s="74"/>
-      <c r="G104" s="76"/>
+      <c r="A104" s="83"/>
+      <c r="B104" s="85"/>
+      <c r="C104" s="62"/>
+      <c r="D104" s="65"/>
+      <c r="E104" s="89"/>
+      <c r="F104" s="68"/>
+      <c r="G104" s="70"/>
       <c r="H104" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I104" s="78"/>
-      <c r="J104" s="71"/>
+      <c r="I104" s="54"/>
+      <c r="J104" s="57"/>
     </row>
     <row r="105" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="54"/>
-      <c r="B105" s="56"/>
-      <c r="C105" s="58"/>
-      <c r="D105" s="66"/>
-      <c r="E105" s="68"/>
+      <c r="A105" s="83"/>
+      <c r="B105" s="85"/>
+      <c r="C105" s="62"/>
+      <c r="D105" s="65"/>
+      <c r="E105" s="97"/>
       <c r="F105" s="15">
         <v>7</v>
       </c>
@@ -4002,15 +4002,15 @@
         <v>80</v>
       </c>
       <c r="H105" s="33"/>
-      <c r="I105" s="79"/>
-      <c r="J105" s="71"/>
+      <c r="I105" s="66"/>
+      <c r="J105" s="57"/>
     </row>
     <row r="106" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="54"/>
-      <c r="B106" s="56"/>
-      <c r="C106" s="58"/>
-      <c r="D106" s="66"/>
-      <c r="E106" s="61"/>
+      <c r="A106" s="83"/>
+      <c r="B106" s="85"/>
+      <c r="C106" s="62"/>
+      <c r="D106" s="65"/>
+      <c r="E106" s="89"/>
       <c r="F106" s="22">
         <v>8</v>
       </c>
@@ -4018,23 +4018,23 @@
         <v>33</v>
       </c>
       <c r="H106" s="34"/>
-      <c r="I106" s="78"/>
-      <c r="J106" s="71"/>
+      <c r="I106" s="54"/>
+      <c r="J106" s="57"/>
     </row>
     <row r="107" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="53">
+      <c r="A107" s="61">
         <v>12</v>
       </c>
-      <c r="B107" s="55" t="s">
+      <c r="B107" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="C107" s="53" t="s">
+      <c r="C107" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="D107" s="59" t="s">
+      <c r="D107" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="E107" s="59" t="s">
+      <c r="E107" s="87" t="s">
         <v>84</v>
       </c>
       <c r="F107" s="9">
@@ -4049,14 +4049,14 @@
       <c r="I107" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J107" s="70"/>
+      <c r="J107" s="56"/>
     </row>
     <row r="108" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="54"/>
-      <c r="B108" s="56"/>
-      <c r="C108" s="58"/>
-      <c r="D108" s="60"/>
-      <c r="E108" s="60"/>
+      <c r="A108" s="83"/>
+      <c r="B108" s="85"/>
+      <c r="C108" s="62"/>
+      <c r="D108" s="88"/>
+      <c r="E108" s="88"/>
       <c r="F108" s="15">
         <v>2</v>
       </c>
@@ -4069,14 +4069,14 @@
       <c r="I108" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J108" s="71"/>
+      <c r="J108" s="57"/>
     </row>
     <row r="109" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A109" s="54"/>
-      <c r="B109" s="56"/>
-      <c r="C109" s="58"/>
-      <c r="D109" s="61"/>
-      <c r="E109" s="61"/>
+      <c r="A109" s="83"/>
+      <c r="B109" s="85"/>
+      <c r="C109" s="62"/>
+      <c r="D109" s="89"/>
+      <c r="E109" s="89"/>
       <c r="F109" s="15">
         <v>3</v>
       </c>
@@ -4087,14 +4087,14 @@
       <c r="I109" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J109" s="71"/>
+      <c r="J109" s="57"/>
     </row>
     <row r="110" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A110" s="54"/>
-      <c r="B110" s="56"/>
-      <c r="C110" s="58"/>
-      <c r="D110" s="61"/>
-      <c r="E110" s="61"/>
+      <c r="A110" s="83"/>
+      <c r="B110" s="85"/>
+      <c r="C110" s="62"/>
+      <c r="D110" s="89"/>
+      <c r="E110" s="89"/>
       <c r="F110" s="15">
         <v>4</v>
       </c>
@@ -4105,14 +4105,14 @@
       <c r="I110" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J110" s="71"/>
+      <c r="J110" s="57"/>
     </row>
     <row r="111" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A111" s="54"/>
-      <c r="B111" s="56"/>
-      <c r="C111" s="58"/>
-      <c r="D111" s="61"/>
-      <c r="E111" s="61"/>
+      <c r="A111" s="83"/>
+      <c r="B111" s="85"/>
+      <c r="C111" s="62"/>
+      <c r="D111" s="89"/>
+      <c r="E111" s="89"/>
       <c r="F111" s="15">
         <v>5</v>
       </c>
@@ -4123,14 +4123,14 @@
       <c r="I111" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J111" s="71"/>
+      <c r="J111" s="57"/>
     </row>
     <row r="112" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="54"/>
-      <c r="B112" s="56"/>
-      <c r="C112" s="58"/>
-      <c r="D112" s="61"/>
-      <c r="E112" s="61"/>
+      <c r="A112" s="83"/>
+      <c r="B112" s="85"/>
+      <c r="C112" s="62"/>
+      <c r="D112" s="89"/>
+      <c r="E112" s="89"/>
       <c r="F112" s="17">
         <v>6</v>
       </c>
@@ -4140,63 +4140,63 @@
       <c r="H112" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I112" s="77" t="s">
+      <c r="I112" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="J112" s="71"/>
+      <c r="J112" s="57"/>
     </row>
     <row r="113" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="54"/>
-      <c r="B113" s="56"/>
-      <c r="C113" s="58"/>
-      <c r="D113" s="61"/>
-      <c r="E113" s="61"/>
-      <c r="F113" s="73">
+      <c r="A113" s="83"/>
+      <c r="B113" s="85"/>
+      <c r="C113" s="62"/>
+      <c r="D113" s="89"/>
+      <c r="E113" s="89"/>
+      <c r="F113" s="67">
         <v>7</v>
       </c>
-      <c r="G113" s="82" t="s">
+      <c r="G113" s="71" t="s">
         <v>73</v>
       </c>
       <c r="H113" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I113" s="78"/>
-      <c r="J113" s="71"/>
+      <c r="I113" s="54"/>
+      <c r="J113" s="57"/>
     </row>
     <row r="114" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A114" s="54"/>
-      <c r="B114" s="56"/>
-      <c r="C114" s="58"/>
-      <c r="D114" s="61"/>
-      <c r="E114" s="61"/>
-      <c r="F114" s="74"/>
-      <c r="G114" s="83"/>
+      <c r="A114" s="83"/>
+      <c r="B114" s="85"/>
+      <c r="C114" s="62"/>
+      <c r="D114" s="89"/>
+      <c r="E114" s="89"/>
+      <c r="F114" s="68"/>
+      <c r="G114" s="72"/>
       <c r="H114" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="I114" s="78"/>
-      <c r="J114" s="71"/>
+      <c r="I114" s="54"/>
+      <c r="J114" s="57"/>
     </row>
     <row r="115" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="54"/>
-      <c r="B115" s="56"/>
-      <c r="C115" s="58"/>
-      <c r="D115" s="61"/>
-      <c r="E115" s="61"/>
-      <c r="F115" s="81"/>
-      <c r="G115" s="84"/>
+      <c r="A115" s="83"/>
+      <c r="B115" s="85"/>
+      <c r="C115" s="62"/>
+      <c r="D115" s="89"/>
+      <c r="E115" s="89"/>
+      <c r="F115" s="74"/>
+      <c r="G115" s="73"/>
       <c r="H115" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I115" s="78"/>
-      <c r="J115" s="71"/>
+      <c r="I115" s="54"/>
+      <c r="J115" s="57"/>
     </row>
     <row r="116" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="54"/>
-      <c r="B116" s="56"/>
-      <c r="C116" s="58"/>
-      <c r="D116" s="61"/>
-      <c r="E116" s="61"/>
+      <c r="A116" s="83"/>
+      <c r="B116" s="85"/>
+      <c r="C116" s="62"/>
+      <c r="D116" s="89"/>
+      <c r="E116" s="89"/>
       <c r="F116" s="21">
         <v>8</v>
       </c>
@@ -4204,21 +4204,21 @@
         <v>33</v>
       </c>
       <c r="H116" s="28"/>
-      <c r="I116" s="78"/>
-      <c r="J116" s="71"/>
+      <c r="I116" s="54"/>
+      <c r="J116" s="57"/>
     </row>
     <row r="117" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="53">
+      <c r="A117" s="61">
         <v>13</v>
       </c>
-      <c r="B117" s="56"/>
-      <c r="C117" s="53" t="s">
+      <c r="B117" s="85"/>
+      <c r="C117" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="D117" s="64" t="s">
+      <c r="D117" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="E117" s="59" t="s">
+      <c r="E117" s="87" t="s">
         <v>89</v>
       </c>
       <c r="F117" s="9">
@@ -4233,14 +4233,14 @@
       <c r="I117" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J117" s="70"/>
+      <c r="J117" s="56"/>
     </row>
     <row r="118" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="54"/>
-      <c r="B118" s="56"/>
-      <c r="C118" s="58"/>
-      <c r="D118" s="65"/>
-      <c r="E118" s="60"/>
+      <c r="A118" s="83"/>
+      <c r="B118" s="85"/>
+      <c r="C118" s="62"/>
+      <c r="D118" s="64"/>
+      <c r="E118" s="88"/>
       <c r="F118" s="15">
         <v>2</v>
       </c>
@@ -4253,14 +4253,14 @@
       <c r="I118" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J118" s="71"/>
+      <c r="J118" s="57"/>
     </row>
     <row r="119" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A119" s="54"/>
-      <c r="B119" s="56"/>
-      <c r="C119" s="58"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="61"/>
+      <c r="A119" s="83"/>
+      <c r="B119" s="85"/>
+      <c r="C119" s="62"/>
+      <c r="D119" s="65"/>
+      <c r="E119" s="89"/>
       <c r="F119" s="15">
         <v>3</v>
       </c>
@@ -4271,14 +4271,14 @@
       <c r="I119" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J119" s="71"/>
+      <c r="J119" s="57"/>
     </row>
     <row r="120" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A120" s="54"/>
-      <c r="B120" s="56"/>
-      <c r="C120" s="58"/>
-      <c r="D120" s="66"/>
-      <c r="E120" s="61"/>
+      <c r="A120" s="83"/>
+      <c r="B120" s="85"/>
+      <c r="C120" s="62"/>
+      <c r="D120" s="65"/>
+      <c r="E120" s="89"/>
       <c r="F120" s="15">
         <v>4</v>
       </c>
@@ -4289,14 +4289,14 @@
       <c r="I120" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J120" s="71"/>
+      <c r="J120" s="57"/>
     </row>
     <row r="121" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A121" s="54"/>
-      <c r="B121" s="56"/>
-      <c r="C121" s="58"/>
-      <c r="D121" s="66"/>
-      <c r="E121" s="61"/>
+      <c r="A121" s="83"/>
+      <c r="B121" s="85"/>
+      <c r="C121" s="62"/>
+      <c r="D121" s="65"/>
+      <c r="E121" s="89"/>
       <c r="F121" s="15">
         <v>5</v>
       </c>
@@ -4307,62 +4307,62 @@
       <c r="I121" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J121" s="71"/>
+      <c r="J121" s="57"/>
     </row>
     <row r="122" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="54"/>
-      <c r="B122" s="56"/>
-      <c r="C122" s="58"/>
-      <c r="D122" s="66"/>
-      <c r="E122" s="61"/>
-      <c r="F122" s="73">
+      <c r="A122" s="83"/>
+      <c r="B122" s="85"/>
+      <c r="C122" s="62"/>
+      <c r="D122" s="65"/>
+      <c r="E122" s="89"/>
+      <c r="F122" s="67">
         <v>6</v>
       </c>
-      <c r="G122" s="75" t="s">
+      <c r="G122" s="69" t="s">
         <v>77</v>
       </c>
       <c r="H122" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="I122" s="77" t="s">
+      <c r="I122" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="J122" s="71"/>
+      <c r="J122" s="57"/>
     </row>
     <row r="123" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="54"/>
-      <c r="B123" s="56"/>
-      <c r="C123" s="58"/>
-      <c r="D123" s="66"/>
-      <c r="E123" s="61"/>
-      <c r="F123" s="74"/>
-      <c r="G123" s="76"/>
+      <c r="A123" s="83"/>
+      <c r="B123" s="85"/>
+      <c r="C123" s="62"/>
+      <c r="D123" s="65"/>
+      <c r="E123" s="89"/>
+      <c r="F123" s="68"/>
+      <c r="G123" s="70"/>
       <c r="H123" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I123" s="78"/>
-      <c r="J123" s="71"/>
+      <c r="I123" s="54"/>
+      <c r="J123" s="57"/>
     </row>
     <row r="124" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="54"/>
-      <c r="B124" s="56"/>
-      <c r="C124" s="58"/>
-      <c r="D124" s="66"/>
-      <c r="E124" s="61"/>
-      <c r="F124" s="74"/>
-      <c r="G124" s="76"/>
+      <c r="A124" s="83"/>
+      <c r="B124" s="85"/>
+      <c r="C124" s="62"/>
+      <c r="D124" s="65"/>
+      <c r="E124" s="89"/>
+      <c r="F124" s="68"/>
+      <c r="G124" s="70"/>
       <c r="H124" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I124" s="78"/>
-      <c r="J124" s="71"/>
+      <c r="I124" s="54"/>
+      <c r="J124" s="57"/>
     </row>
     <row r="125" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="54"/>
-      <c r="B125" s="56"/>
-      <c r="C125" s="58"/>
-      <c r="D125" s="66"/>
-      <c r="E125" s="68"/>
+      <c r="A125" s="83"/>
+      <c r="B125" s="85"/>
+      <c r="C125" s="62"/>
+      <c r="D125" s="65"/>
+      <c r="E125" s="97"/>
       <c r="F125" s="15">
         <v>7</v>
       </c>
@@ -4372,15 +4372,15 @@
       <c r="H125" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="I125" s="79"/>
-      <c r="J125" s="71"/>
+      <c r="I125" s="66"/>
+      <c r="J125" s="57"/>
     </row>
     <row r="126" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="62"/>
-      <c r="B126" s="57"/>
-      <c r="C126" s="63"/>
-      <c r="D126" s="67"/>
-      <c r="E126" s="69"/>
+      <c r="A126" s="98"/>
+      <c r="B126" s="90"/>
+      <c r="C126" s="99"/>
+      <c r="D126" s="100"/>
+      <c r="E126" s="101"/>
       <c r="F126" s="40">
         <v>8</v>
       </c>
@@ -4388,76 +4388,28 @@
         <v>33</v>
       </c>
       <c r="H126" s="42"/>
-      <c r="I126" s="80"/>
-      <c r="J126" s="72"/>
+      <c r="I126" s="103"/>
+      <c r="J126" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="I50:I53"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="J25:J34"/>
-    <mergeCell ref="J35:J44"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="J65:J74"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="J75:J80"/>
-    <mergeCell ref="G60:G63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="C65:C74"/>
-    <mergeCell ref="D65:D74"/>
-    <mergeCell ref="J97:J106"/>
-    <mergeCell ref="I102:I106"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="J87:J96"/>
-    <mergeCell ref="G93:G95"/>
-    <mergeCell ref="F93:F95"/>
-    <mergeCell ref="I92:I96"/>
-    <mergeCell ref="J81:J86"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="B5:B14"/>
-    <mergeCell ref="C5:C14"/>
-    <mergeCell ref="D5:D14"/>
-    <mergeCell ref="E5:E14"/>
-    <mergeCell ref="J5:J14"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="D35:D44"/>
-    <mergeCell ref="E35:E44"/>
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="I70:I73"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="A65:A74"/>
-    <mergeCell ref="B15:B74"/>
-    <mergeCell ref="C55:C64"/>
-    <mergeCell ref="D55:D64"/>
-    <mergeCell ref="E55:E64"/>
-    <mergeCell ref="J55:J64"/>
-    <mergeCell ref="F60:F63"/>
-    <mergeCell ref="D15:D24"/>
-    <mergeCell ref="E15:E24"/>
-    <mergeCell ref="J15:J24"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J45:J54"/>
-    <mergeCell ref="F50:F53"/>
-    <mergeCell ref="G50:G53"/>
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="C25:C34"/>
-    <mergeCell ref="D25:D34"/>
-    <mergeCell ref="E25:E34"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="A107:A116"/>
+    <mergeCell ref="B107:B126"/>
+    <mergeCell ref="C107:C116"/>
+    <mergeCell ref="D107:D116"/>
+    <mergeCell ref="A117:A126"/>
+    <mergeCell ref="C117:C126"/>
+    <mergeCell ref="D117:D126"/>
+    <mergeCell ref="E117:E126"/>
+    <mergeCell ref="J117:J126"/>
+    <mergeCell ref="F122:F124"/>
+    <mergeCell ref="G122:G124"/>
+    <mergeCell ref="I122:I126"/>
+    <mergeCell ref="E107:E116"/>
+    <mergeCell ref="J107:J116"/>
+    <mergeCell ref="I112:I116"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="G113:G115"/>
     <mergeCell ref="A75:A80"/>
     <mergeCell ref="B75:B80"/>
     <mergeCell ref="C75:C80"/>
@@ -4482,23 +4434,71 @@
     <mergeCell ref="E81:E86"/>
     <mergeCell ref="A87:A96"/>
     <mergeCell ref="C87:C96"/>
-    <mergeCell ref="A107:A116"/>
-    <mergeCell ref="B107:B126"/>
-    <mergeCell ref="C107:C116"/>
-    <mergeCell ref="D107:D116"/>
-    <mergeCell ref="A117:A126"/>
-    <mergeCell ref="C117:C126"/>
-    <mergeCell ref="D117:D126"/>
-    <mergeCell ref="E117:E126"/>
-    <mergeCell ref="J117:J126"/>
-    <mergeCell ref="F122:F124"/>
-    <mergeCell ref="G122:G124"/>
-    <mergeCell ref="I122:I126"/>
-    <mergeCell ref="E107:E116"/>
-    <mergeCell ref="J107:J116"/>
-    <mergeCell ref="I112:I116"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="A65:A74"/>
+    <mergeCell ref="B15:B74"/>
+    <mergeCell ref="C55:C64"/>
+    <mergeCell ref="D55:D64"/>
+    <mergeCell ref="E55:E64"/>
+    <mergeCell ref="J55:J64"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="D15:D24"/>
+    <mergeCell ref="E15:E24"/>
+    <mergeCell ref="J15:J24"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J45:J54"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="G50:G53"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="C25:C34"/>
+    <mergeCell ref="D25:D34"/>
+    <mergeCell ref="E25:E34"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="B5:B14"/>
+    <mergeCell ref="C5:C14"/>
+    <mergeCell ref="D5:D14"/>
+    <mergeCell ref="E5:E14"/>
+    <mergeCell ref="J5:J14"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="D35:D44"/>
+    <mergeCell ref="E35:E44"/>
+    <mergeCell ref="C65:C74"/>
+    <mergeCell ref="D65:D74"/>
+    <mergeCell ref="J97:J106"/>
+    <mergeCell ref="I102:I106"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="J87:J96"/>
+    <mergeCell ref="G93:G95"/>
+    <mergeCell ref="F93:F95"/>
+    <mergeCell ref="I92:I96"/>
+    <mergeCell ref="J81:J86"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="I50:I53"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="J25:J34"/>
+    <mergeCell ref="J35:J44"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="J65:J74"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="J75:J80"/>
+    <mergeCell ref="G60:G63"/>
+    <mergeCell ref="I60:I63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
@@ -4541,7 +4541,7 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -4557,18 +4557,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="38"/>
@@ -4615,33 +4615,33 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="53">
+      <c r="A5" s="61">
         <v>1</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="87" t="s">
         <v>97</v>
       </c>
       <c r="F5" s="9">
@@ -4656,14 +4656,14 @@
       <c r="I5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="70"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="60"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="88"/>
       <c r="F6" s="12">
         <v>2</v>
       </c>
@@ -4676,14 +4676,14 @@
       <c r="I6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="71"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="61"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="12">
         <v>3</v>
       </c>
@@ -4694,14 +4694,14 @@
       <c r="I7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="71"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="61"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="12">
         <v>4</v>
       </c>
@@ -4712,14 +4712,14 @@
       <c r="I8" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J8" s="71"/>
+      <c r="J8" s="57"/>
     </row>
     <row r="9" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="61"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="12">
         <v>5</v>
       </c>
@@ -4730,14 +4730,14 @@
       <c r="I9" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="71"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="105"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="109"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="108"/>
       <c r="F10" s="45">
         <v>6</v>
       </c>
@@ -4748,20 +4748,20 @@
       <c r="I10" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="104"/>
+      <c r="J10" s="109"/>
     </row>
     <row r="11" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="53">
+      <c r="A11" s="61">
         <v>2</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="55" t="s">
+      <c r="B11" s="85"/>
+      <c r="C11" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="87" t="s">
         <v>97</v>
       </c>
       <c r="F11" s="9">
@@ -4776,14 +4776,14 @@
       <c r="I11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="70"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="60"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="88"/>
       <c r="F12" s="12">
         <v>2</v>
       </c>
@@ -4796,14 +4796,14 @@
       <c r="I12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="71"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="61"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="89"/>
       <c r="F13" s="12">
         <v>3</v>
       </c>
@@ -4814,14 +4814,14 @@
       <c r="I13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="71"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="61"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="89"/>
       <c r="F14" s="12">
         <v>4</v>
       </c>
@@ -4832,14 +4832,14 @@
       <c r="I14" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J14" s="71"/>
+      <c r="J14" s="57"/>
     </row>
     <row r="15" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="61"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="89"/>
       <c r="F15" s="12">
         <v>5</v>
       </c>
@@ -4847,17 +4847,17 @@
         <v>106</v>
       </c>
       <c r="H15" s="37"/>
-      <c r="I15" s="77" t="s">
+      <c r="I15" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="71"/>
+      <c r="J15" s="57"/>
     </row>
     <row r="16" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="61"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="89"/>
       <c r="F16" s="39">
         <v>6</v>
       </c>
@@ -4865,15 +4865,15 @@
         <v>107</v>
       </c>
       <c r="H16" s="37"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="71"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="105"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="109"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="108"/>
       <c r="F17" s="45">
         <v>7</v>
       </c>
@@ -4884,22 +4884,22 @@
       <c r="I17" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="J17" s="104"/>
+      <c r="J17" s="109"/>
     </row>
     <row r="18" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="53">
+      <c r="A18" s="61">
         <v>3</v>
       </c>
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="110" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="64" t="s">
+      <c r="D18" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="87" t="s">
         <v>111</v>
       </c>
       <c r="F18" s="9">
@@ -4914,14 +4914,14 @@
       <c r="I18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="70"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="60"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="88"/>
       <c r="F19" s="12">
         <v>2</v>
       </c>
@@ -4934,14 +4934,14 @@
       <c r="I19" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="71"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="61"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="89"/>
       <c r="F20" s="12">
         <v>3</v>
       </c>
@@ -4952,14 +4952,14 @@
       <c r="I20" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="71"/>
+      <c r="J20" s="57"/>
     </row>
     <row r="21" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="61"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="89"/>
       <c r="F21" s="12">
         <v>4</v>
       </c>
@@ -4970,14 +4970,14 @@
       <c r="I21" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="71"/>
+      <c r="J21" s="57"/>
     </row>
     <row r="22" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="85"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="61"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="89"/>
       <c r="F22" s="12">
         <v>5</v>
       </c>
@@ -4985,17 +4985,17 @@
         <v>112</v>
       </c>
       <c r="H22" s="37"/>
-      <c r="I22" s="77" t="s">
+      <c r="I22" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="71"/>
+      <c r="J22" s="57"/>
     </row>
     <row r="23" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="61"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="89"/>
       <c r="F23" s="39">
         <v>6</v>
       </c>
@@ -5003,15 +5003,15 @@
         <v>107</v>
       </c>
       <c r="H23" s="37"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="71"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="57"/>
     </row>
     <row r="24" spans="1:10" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="105"/>
-      <c r="B24" s="106"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="109"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="108"/>
       <c r="F24" s="45">
         <v>7</v>
       </c>
@@ -5022,22 +5022,22 @@
       <c r="I24" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="J24" s="104"/>
+      <c r="J24" s="109"/>
     </row>
     <row r="25" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="53">
+      <c r="A25" s="61">
         <v>4</v>
       </c>
-      <c r="B25" s="111" t="s">
+      <c r="B25" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="87" t="s">
         <v>111</v>
       </c>
       <c r="F25" s="9">
@@ -5052,14 +5052,14 @@
       <c r="I25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="70"/>
+      <c r="J25" s="56"/>
     </row>
     <row r="26" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="60"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="88"/>
       <c r="F26" s="12">
         <v>2</v>
       </c>
@@ -5072,14 +5072,14 @@
       <c r="I26" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="71"/>
+      <c r="J26" s="57"/>
     </row>
     <row r="27" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="85"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="61"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="89"/>
       <c r="F27" s="12">
         <v>3</v>
       </c>
@@ -5090,14 +5090,14 @@
       <c r="I27" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="71"/>
+      <c r="J27" s="57"/>
     </row>
     <row r="28" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="61"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="89"/>
       <c r="F28" s="12">
         <v>4</v>
       </c>
@@ -5108,14 +5108,14 @@
       <c r="I28" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="J28" s="71"/>
+      <c r="J28" s="57"/>
     </row>
     <row r="29" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="61"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="89"/>
       <c r="F29" s="12">
         <v>5</v>
       </c>
@@ -5126,14 +5126,14 @@
       <c r="I29" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="J29" s="110"/>
+      <c r="J29" s="111"/>
     </row>
     <row r="30" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="61"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="89"/>
       <c r="F30" s="39">
         <v>6</v>
       </c>
@@ -5144,14 +5144,14 @@
       <c r="I30" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="J30" s="110"/>
+      <c r="J30" s="111"/>
     </row>
     <row r="31" spans="1:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="105"/>
-      <c r="B31" s="106"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="109"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="105"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="108"/>
       <c r="F31" s="45">
         <v>7</v>
       </c>
@@ -5162,22 +5162,22 @@
       <c r="I31" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="104"/>
+      <c r="J31" s="109"/>
     </row>
     <row r="32" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="53">
+      <c r="A32" s="61">
         <v>5</v>
       </c>
-      <c r="B32" s="111" t="s">
+      <c r="B32" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="64" t="s">
+      <c r="D32" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="87" t="s">
         <v>121</v>
       </c>
       <c r="F32" s="9">
@@ -5192,14 +5192,14 @@
       <c r="I32" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="70"/>
+      <c r="J32" s="56"/>
     </row>
     <row r="33" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="54"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="60"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="88"/>
       <c r="F33" s="12">
         <v>2</v>
       </c>
@@ -5212,14 +5212,14 @@
       <c r="I33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="71"/>
+      <c r="J33" s="57"/>
     </row>
     <row r="34" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="54"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="61"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="89"/>
       <c r="F34" s="12">
         <v>3</v>
       </c>
@@ -5230,14 +5230,14 @@
       <c r="I34" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="71"/>
+      <c r="J34" s="57"/>
     </row>
     <row r="35" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="54"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="61"/>
+      <c r="A35" s="83"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="89"/>
       <c r="F35" s="12">
         <v>4</v>
       </c>
@@ -5248,14 +5248,14 @@
       <c r="I35" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J35" s="71"/>
+      <c r="J35" s="57"/>
     </row>
     <row r="36" spans="1:10" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="105"/>
-      <c r="B36" s="106"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="108"/>
-      <c r="E36" s="109"/>
+      <c r="A36" s="104"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="107"/>
+      <c r="E36" s="108"/>
       <c r="F36" s="45">
         <v>5</v>
       </c>
@@ -5269,19 +5269,19 @@
       <c r="J36" s="112"/>
     </row>
     <row r="37" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="53">
+      <c r="A37" s="61">
         <v>6</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="64" t="s">
+      <c r="D37" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="59" t="s">
+      <c r="E37" s="87" t="s">
         <v>127</v>
       </c>
       <c r="F37" s="9">
@@ -5296,14 +5296,14 @@
       <c r="I37" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="70"/>
+      <c r="J37" s="56"/>
     </row>
     <row r="38" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="54"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="60"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="88"/>
       <c r="F38" s="12">
         <v>2</v>
       </c>
@@ -5316,14 +5316,14 @@
       <c r="I38" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J38" s="71"/>
+      <c r="J38" s="57"/>
     </row>
     <row r="39" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="54"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="61"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="89"/>
       <c r="F39" s="12">
         <v>3</v>
       </c>
@@ -5334,14 +5334,14 @@
       <c r="I39" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J39" s="71"/>
+      <c r="J39" s="57"/>
     </row>
     <row r="40" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="54"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="61"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="89"/>
       <c r="F40" s="12">
         <v>4</v>
       </c>
@@ -5352,14 +5352,14 @@
       <c r="I40" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J40" s="71"/>
+      <c r="J40" s="57"/>
     </row>
     <row r="41" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="54"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="61"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="89"/>
       <c r="F41" s="12">
         <v>5</v>
       </c>
@@ -5370,14 +5370,14 @@
       <c r="I41" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="J41" s="71"/>
+      <c r="J41" s="57"/>
     </row>
     <row r="42" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="105"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="107"/>
-      <c r="D42" s="108"/>
-      <c r="E42" s="109"/>
+      <c r="A42" s="104"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="107"/>
+      <c r="E42" s="108"/>
       <c r="F42" s="45">
         <v>6</v>
       </c>
@@ -5388,20 +5388,20 @@
       <c r="I42" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="J42" s="104"/>
+      <c r="J42" s="109"/>
     </row>
     <row r="43" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="53">
+      <c r="A43" s="61">
         <v>7</v>
       </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="55" t="s">
+      <c r="B43" s="85"/>
+      <c r="C43" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="64" t="s">
+      <c r="D43" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="59" t="s">
+      <c r="E43" s="87" t="s">
         <v>127</v>
       </c>
       <c r="F43" s="9">
@@ -5416,14 +5416,14 @@
       <c r="I43" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J43" s="70"/>
+      <c r="J43" s="56"/>
     </row>
     <row r="44" spans="1:10" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="54"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="60"/>
+      <c r="A44" s="83"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="88"/>
       <c r="F44" s="12">
         <v>2</v>
       </c>
@@ -5436,14 +5436,14 @@
       <c r="I44" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J44" s="71"/>
+      <c r="J44" s="57"/>
     </row>
     <row r="45" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="54"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="61"/>
+      <c r="A45" s="83"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="89"/>
       <c r="F45" s="12">
         <v>3</v>
       </c>
@@ -5454,14 +5454,14 @@
       <c r="I45" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J45" s="71"/>
+      <c r="J45" s="57"/>
     </row>
     <row r="46" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="54"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="85"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="61"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="89"/>
       <c r="F46" s="12">
         <v>4</v>
       </c>
@@ -5472,14 +5472,14 @@
       <c r="I46" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J46" s="71"/>
+      <c r="J46" s="57"/>
     </row>
     <row r="47" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="54"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="61"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="89"/>
       <c r="F47" s="12">
         <v>5</v>
       </c>
@@ -5490,14 +5490,14 @@
       <c r="I47" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="J47" s="71"/>
+      <c r="J47" s="57"/>
     </row>
     <row r="48" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="105"/>
-      <c r="B48" s="106"/>
-      <c r="C48" s="107"/>
-      <c r="D48" s="108"/>
-      <c r="E48" s="109"/>
+      <c r="A48" s="104"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="106"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="108"/>
       <c r="F48" s="45">
         <v>6</v>
       </c>
@@ -5508,10 +5508,40 @@
       <c r="I48" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="J48" s="104"/>
+      <c r="J48" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="J43:J48"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B48"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="J37:J42"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="J18:J24"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="J25:J31"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="E18:E24"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:A10"/>
@@ -5526,36 +5556,6 @@
     <mergeCell ref="E11:E17"/>
     <mergeCell ref="J11:J17"/>
     <mergeCell ref="I15:I16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="J18:J24"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="J25:J31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="J32:J36"/>
-    <mergeCell ref="J43:J48"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B48"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="J37:J42"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="E43:E48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>

</xml_diff>